<commit_message>
New Queries (details below)
- Having
- EXISTS
- String Operations
- (LEFT) OUTER JOIN
- ALTER TABLE (don't run it)
</commit_message>
<xml_diff>
--- a/Database Grading Criteria.xlsx
+++ b/Database Grading Criteria.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gokaytoga/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/canmizrakli/Desktop/Aviation-Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EFFDE12-8767-2A41-B9E3-811B4823AE88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F166B451-03DA-F342-A22C-142EA3089A99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="3740" windowWidth="28820" windowHeight="15380" xr2:uid="{F29DC715-F1A0-4C47-8F05-B76EC17FA4A9}"/>
+    <workbookView xWindow="580" yWindow="2800" windowWidth="28820" windowHeight="15380" xr2:uid="{F29DC715-F1A0-4C47-8F05-B76EC17FA4A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="54">
   <si>
     <t>Grading Element</t>
   </si>
@@ -192,13 +192,19 @@
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>used left outer join fyi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -242,10 +248,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Helvetica"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -301,7 +314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -319,6 +332,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -633,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDA35D2A-57AC-4043-9C00-05563D535B26}">
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" zoomScale="194" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -742,7 +756,9 @@
       <c r="B10" s="3">
         <v>2</v>
       </c>
-      <c r="C10" s="8"/>
+      <c r="C10" s="9" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
@@ -804,7 +820,7 @@
       </c>
       <c r="C16" s="8"/>
     </row>
-    <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>17</v>
       </c>
@@ -815,7 +831,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>18</v>
       </c>
@@ -824,7 +840,7 @@
       </c>
       <c r="C18" s="8"/>
     </row>
-    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>19</v>
       </c>
@@ -833,7 +849,7 @@
       </c>
       <c r="C19" s="8"/>
     </row>
-    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>20</v>
       </c>
@@ -844,7 +860,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>21</v>
       </c>
@@ -855,16 +871,21 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="3">
         <v>2</v>
       </c>
-      <c r="C22" s="8"/>
-    </row>
-    <row r="23" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="C22" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>23</v>
       </c>
@@ -873,7 +894,7 @@
       </c>
       <c r="C23" s="8"/>
     </row>
-    <row r="24" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>24</v>
       </c>
@@ -882,7 +903,7 @@
       </c>
       <c r="C24" s="8"/>
     </row>
-    <row r="25" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>25</v>
       </c>
@@ -893,7 +914,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>26</v>
       </c>
@@ -904,7 +925,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>27</v>
       </c>
@@ -915,7 +936,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>28</v>
       </c>
@@ -926,7 +947,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>29</v>
       </c>
@@ -937,7 +958,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>30</v>
       </c>
@@ -948,7 +969,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>31</v>
       </c>
@@ -959,7 +980,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>32</v>
       </c>
@@ -977,7 +998,9 @@
       <c r="B33" s="3">
         <v>2</v>
       </c>
-      <c r="C33" s="8"/>
+      <c r="C33" s="9" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="34" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
@@ -986,7 +1009,9 @@
       <c r="B34" s="3">
         <v>2</v>
       </c>
-      <c r="C34" s="8"/>
+      <c r="C34" s="9" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="35" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
@@ -1116,7 +1141,9 @@
       <c r="B46" s="3">
         <v>2</v>
       </c>
-      <c r="C46" s="8"/>
+      <c r="C46" s="9" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="47" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">

</xml_diff>

<commit_message>
All query requirements have been completed
</commit_message>
<xml_diff>
--- a/Database Grading Criteria.xlsx
+++ b/Database Grading Criteria.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gokaytoga/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/canmizrakli/Desktop/Aviation-Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E791DBA-B8BD-954B-A6AE-42AA0EBED161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07206418-62C3-D84F-890A-00AF3127F49D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="3740" windowWidth="28820" windowHeight="15380" xr2:uid="{F29DC715-F1A0-4C47-8F05-B76EC17FA4A9}"/>
+    <workbookView xWindow="580" yWindow="2720" windowWidth="28820" windowHeight="15380" xr2:uid="{F29DC715-F1A0-4C47-8F05-B76EC17FA4A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="53">
   <si>
     <t>Grading Element</t>
   </si>
@@ -638,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDA35D2A-57AC-4043-9C00-05563D535B26}">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -833,7 +833,9 @@
       <c r="B18" s="3">
         <v>1</v>
       </c>
-      <c r="C18" s="8"/>
+      <c r="C18" s="7" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
@@ -842,7 +844,9 @@
       <c r="B19" s="3">
         <v>1</v>
       </c>
-      <c r="C19" s="8"/>
+      <c r="C19" s="7" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
@@ -884,7 +888,9 @@
       <c r="B23" s="3">
         <v>2</v>
       </c>
-      <c r="C23" s="8"/>
+      <c r="C23" s="7" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="24" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
@@ -893,7 +899,9 @@
       <c r="B24" s="3">
         <v>2</v>
       </c>
-      <c r="C24" s="8"/>
+      <c r="C24" s="7" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="25" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">

</xml_diff>